<commit_message>
table border is fixed
</commit_message>
<xml_diff>
--- a/Anastasia.xlsx
+++ b/Anastasia.xlsx
@@ -121,7 +121,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -129,12 +129,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -417,13 +433,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="11.44140625" customWidth="1"/>
     <col min="3" max="3" width="22.21875" customWidth="1"/>
     <col min="4" max="4" width="32.88671875" customWidth="1"/>
@@ -431,126 +447,125 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E7"/>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>